<commit_message>
documentos de apresentação atualizados
</commit_message>
<xml_diff>
--- a/Documentação/Homologacao  v1.xlsx
+++ b/Documentação/Homologacao  v1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\SenSolutions\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Fernando\Desktop\Meus Arquivos\Faculdade\Bandtec\1Semestre\SenSolutions\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B61F5B-D3CB-4AD6-8779-728680B965B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="675"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
@@ -23,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>move0011</author>
   </authors>
   <commentList>
-    <comment ref="I19" authorId="0" shapeId="0">
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -442,7 +443,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
@@ -1273,6 +1274,65 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="12" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1297,50 +1357,9 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1350,24 +1369,6 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1401,21 +1402,21 @@
     </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Background" xfId="1"/>
-    <cellStyle name="Card" xfId="2"/>
-    <cellStyle name="Card B" xfId="3"/>
-    <cellStyle name="Card BL" xfId="4"/>
-    <cellStyle name="Card BR" xfId="5"/>
-    <cellStyle name="Card L" xfId="6"/>
-    <cellStyle name="Card R" xfId="7"/>
-    <cellStyle name="Card T" xfId="8"/>
-    <cellStyle name="Card TL" xfId="9"/>
-    <cellStyle name="Card TR" xfId="10"/>
-    <cellStyle name="Column Header" xfId="11"/>
+    <cellStyle name="Background" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Card" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Card B" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Card BL" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Card BR" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Card L" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Card R" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Card T" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Card TL" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Card TR" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Column Header" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Hiperlink" xfId="12" builtinId="8"/>
-    <cellStyle name="Input" xfId="13"/>
+    <cellStyle name="Input" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="14"/>
+    <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1515,7 +1516,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1559,7 +1566,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagem 7"/>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1591,19 +1604,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>163285</xdr:colOff>
+      <xdr:colOff>190499</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>258536</xdr:rowOff>
+      <xdr:rowOff>503465</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2911928</xdr:colOff>
+      <xdr:colOff>2939142</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>2054679</xdr:rowOff>
+      <xdr:rowOff>1973036</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagem 8"/>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1622,8 +1641,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11538856" y="6926036"/>
-          <a:ext cx="2748643" cy="1796143"/>
+          <a:off x="11566070" y="7170965"/>
+          <a:ext cx="2748643" cy="1469571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1652,7 +1671,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagem 4"/>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1696,7 +1721,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagem 5"/>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1740,7 +1771,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagem 6"/>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1789,7 +1826,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagem 4"/>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1833,7 +1876,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagem 5"/>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1941,6 +1990,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1976,6 +2042,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2151,10 +2234,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C22" sqref="C22:D22"/>
     </sheetView>
   </sheetViews>
@@ -2192,13 +2275,13 @@
     </row>
     <row r="2" spans="1:20" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51"/>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="80"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="97"/>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -2208,11 +2291,11 @@
     </row>
     <row r="3" spans="1:20" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="83"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="100"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
@@ -2239,10 +2322,10 @@
       <c r="B5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
+      <c r="D5" s="102"/>
       <c r="E5" s="26"/>
       <c r="F5" s="27"/>
       <c r="G5" s="26"/>
@@ -2257,10 +2340,10 @@
       <c r="B6" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="84">
+      <c r="C6" s="101">
         <v>1001</v>
       </c>
-      <c r="D6" s="85"/>
+      <c r="D6" s="102"/>
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
       <c r="G6" s="26"/>
@@ -2275,10 +2358,10 @@
       <c r="B7" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="101" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="85"/>
+      <c r="D7" s="102"/>
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
       <c r="G7" s="26"/>
@@ -2293,10 +2376,10 @@
       <c r="B8" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="85"/>
+      <c r="D8" s="102"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
       <c r="G8" s="26"/>
@@ -2311,10 +2394,10 @@
       <c r="B9" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="88">
+      <c r="C9" s="103">
         <v>43613</v>
       </c>
-      <c r="D9" s="85"/>
+      <c r="D9" s="102"/>
       <c r="E9" s="26"/>
       <c r="F9" s="27"/>
       <c r="G9" s="26"/>
@@ -2340,16 +2423,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="101"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="106"/>
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
       <c r="L11" s="22"/>
@@ -2361,14 +2444,14 @@
       <c r="B12" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="93" t="s">
+      <c r="C12" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="94"/>
-      <c r="E12" s="93" t="s">
+      <c r="D12" s="87"/>
+      <c r="E12" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="94"/>
+      <c r="F12" s="87"/>
       <c r="G12" s="70" t="s">
         <v>24</v>
       </c>
@@ -2391,14 +2474,14 @@
       <c r="B13" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="89" t="s">
+      <c r="D13" s="80"/>
+      <c r="E13" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="95"/>
+      <c r="F13" s="88"/>
       <c r="G13" s="62" t="s">
         <v>104</v>
       </c>
@@ -2421,14 +2504,14 @@
       <c r="B14" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="106"/>
-      <c r="E14" s="96" t="s">
+      <c r="D14" s="94"/>
+      <c r="E14" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="97"/>
+      <c r="F14" s="90"/>
       <c r="G14" s="72" t="s">
         <v>106</v>
       </c>
@@ -2451,14 +2534,14 @@
       <c r="B15" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="86" t="s">
+      <c r="D15" s="80"/>
+      <c r="E15" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="98"/>
+      <c r="F15" s="81"/>
       <c r="G15" s="62" t="s">
         <v>104</v>
       </c>
@@ -2481,10 +2564,10 @@
       <c r="B16" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="86"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="98"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="81"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
@@ -2516,17 +2599,17 @@
     </row>
     <row r="18" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="53"/>
-      <c r="B18" s="102" t="s">
+      <c r="B18" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="103"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="103"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
     </row>
@@ -2535,18 +2618,18 @@
       <c r="B19" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="92"/>
-      <c r="E19" s="91" t="s">
+      <c r="D19" s="85"/>
+      <c r="E19" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="92"/>
-      <c r="G19" s="91" t="s">
+      <c r="F19" s="85"/>
+      <c r="G19" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="92"/>
+      <c r="H19" s="85"/>
       <c r="I19" s="69" t="s">
         <v>26</v>
       </c>
@@ -2565,18 +2648,18 @@
       <c r="B20" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="87"/>
-      <c r="E20" s="86" t="s">
+      <c r="D20" s="80"/>
+      <c r="E20" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="87"/>
-      <c r="G20" s="86" t="s">
+      <c r="F20" s="80"/>
+      <c r="G20" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="87"/>
+      <c r="H20" s="80"/>
       <c r="I20" s="63" t="s">
         <v>109</v>
       </c>
@@ -2595,18 +2678,18 @@
       <c r="B21" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="104"/>
-      <c r="E21" s="89" t="s">
+      <c r="D21" s="79"/>
+      <c r="E21" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="G21" s="89" t="s">
+      <c r="F21" s="83"/>
+      <c r="G21" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="90"/>
+      <c r="H21" s="83"/>
       <c r="I21" s="64" t="s">
         <v>109</v>
       </c>
@@ -2625,18 +2708,18 @@
       <c r="B22" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="104"/>
-      <c r="E22" s="89" t="s">
+      <c r="D22" s="79"/>
+      <c r="E22" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="90"/>
-      <c r="G22" s="89" t="s">
+      <c r="F22" s="83"/>
+      <c r="G22" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="90"/>
+      <c r="H22" s="83"/>
       <c r="I22" s="64" t="s">
         <v>109</v>
       </c>
@@ -2653,12 +2736,12 @@
     <row r="23" spans="1:21" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="52"/>
       <c r="B23" s="61"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="104"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="79"/>
       <c r="I23" s="64"/>
       <c r="J23" s="62"/>
       <c r="K23" s="25"/>
@@ -2804,16 +2887,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:I11"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
@@ -2828,25 +2911,25 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Não Iniciado, Em andamento, Concluído, Pendente"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J20:J23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J20:J23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Não testado,Testado- NÃO OK,Testado - OK"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I23" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Essencial, Importante, Desejável"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2857,10 +2940,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -3240,8 +3323,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -3254,7 +3337,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -3637,8 +3720,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -3651,7 +3734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -4014,8 +4097,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -4028,7 +4111,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">

</xml_diff>

<commit_message>
Atualização da apresentação e normalização de documentos
</commit_message>
<xml_diff>
--- a/Documentação/Homologacao  v1.xlsx
+++ b/Documentação/Homologacao  v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Fernando\Desktop\Meus Arquivos\Faculdade\Bandtec\1Semestre\SenSolutions\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Fernando\Desktop\Meus Arquivos\Faculdade\Bandtec\1Semestre\PI\SenSolutions\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B61F5B-D3CB-4AD6-8779-728680B965B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CF3FEA-59AC-4765-AD93-47797C51C4EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -669,8 +669,52 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Panton Light Caps"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Panton Light Caps"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Panton Light Caps"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Panton Light Caps"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Panton Light Caps"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Panton Light Caps"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -731,8 +775,20 @@
         <bgColor indexed="26"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -967,6 +1023,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0">
@@ -1015,7 +1115,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1223,16 +1323,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1242,9 +1332,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1268,63 +1355,76 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="12" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1333,42 +1433,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1399,6 +1463,114 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="38" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -2237,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2246,9 +2418,13 @@
     <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="16.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
-    <col min="7" max="10" width="16.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" style="2" customWidth="1"/>
     <col min="12" max="12" width="20.5703125" style="2" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" style="2" customWidth="1"/>
@@ -2275,13 +2451,13 @@
     </row>
     <row r="2" spans="1:20" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51"/>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="97"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="75"/>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -2291,11 +2467,11 @@
     </row>
     <row r="3" spans="1:20" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="100"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
@@ -2322,10 +2498,10 @@
       <c r="B5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="102"/>
+      <c r="D5" s="80"/>
       <c r="E5" s="26"/>
       <c r="F5" s="27"/>
       <c r="G5" s="26"/>
@@ -2340,10 +2516,10 @@
       <c r="B6" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="101">
+      <c r="C6" s="79">
         <v>1001</v>
       </c>
-      <c r="D6" s="102"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
       <c r="G6" s="26"/>
@@ -2358,10 +2534,10 @@
       <c r="B7" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="101" t="s">
+      <c r="C7" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="102"/>
+      <c r="D7" s="80"/>
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
       <c r="G7" s="26"/>
@@ -2376,10 +2552,10 @@
       <c r="B8" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="101" t="s">
+      <c r="C8" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="102"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
       <c r="G8" s="26"/>
@@ -2394,10 +2570,10 @@
       <c r="B9" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="103">
+      <c r="C9" s="83">
         <v>43613</v>
       </c>
-      <c r="D9" s="102"/>
+      <c r="D9" s="80"/>
       <c r="E9" s="26"/>
       <c r="F9" s="27"/>
       <c r="G9" s="26"/>
@@ -2423,16 +2599,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
-      <c r="B11" s="104" t="s">
+      <c r="B11" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="106"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="86"/>
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
       <c r="L11" s="22"/>
@@ -2441,24 +2617,24 @@
     </row>
     <row r="12" spans="1:20" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="52"/>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="87"/>
-      <c r="E12" s="86" t="s">
+      <c r="D12" s="89"/>
+      <c r="E12" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="87"/>
-      <c r="G12" s="70" t="s">
+      <c r="F12" s="89"/>
+      <c r="G12" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="70" t="s">
+      <c r="H12" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="70" t="s">
+      <c r="I12" s="66" t="s">
         <v>29</v>
       </c>
       <c r="J12" s="60"/>
@@ -2474,18 +2650,18 @@
       <c r="B13" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="80"/>
-      <c r="E13" s="82" t="s">
+      <c r="D13" s="82"/>
+      <c r="E13" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="88"/>
+      <c r="F13" s="90"/>
       <c r="G13" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="H13" s="74">
+      <c r="H13" s="70">
         <v>43619</v>
       </c>
       <c r="I13" s="62" t="s">
@@ -2501,24 +2677,24 @@
     </row>
     <row r="14" spans="1:20" s="4" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52"/>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="93" t="s">
+      <c r="C14" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="94"/>
-      <c r="E14" s="89" t="s">
+      <c r="D14" s="95"/>
+      <c r="E14" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="90"/>
-      <c r="G14" s="72" t="s">
+      <c r="F14" s="92"/>
+      <c r="G14" s="68" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="75">
+      <c r="H14" s="71">
         <v>43619</v>
       </c>
-      <c r="I14" s="72" t="s">
+      <c r="I14" s="68" t="s">
         <v>105</v>
       </c>
       <c r="J14" s="60"/>
@@ -2534,18 +2710,18 @@
       <c r="B15" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="78" t="s">
+      <c r="D15" s="82"/>
+      <c r="E15" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="81"/>
+      <c r="F15" s="93"/>
       <c r="G15" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="H15" s="74">
+      <c r="H15" s="70">
         <v>43619</v>
       </c>
       <c r="I15" s="62" t="s">
@@ -2564,10 +2740,10 @@
       <c r="B16" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="93"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
@@ -2597,43 +2773,43 @@
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
     </row>
-    <row r="18" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="53"/>
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
+      <c r="C18" s="135"/>
+      <c r="D18" s="135"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="135"/>
+      <c r="J18" s="135"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="52"/>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="84" t="s">
+      <c r="D19" s="133"/>
+      <c r="E19" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="85"/>
-      <c r="G19" s="84" t="s">
+      <c r="F19" s="133"/>
+      <c r="G19" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="85"/>
-      <c r="I19" s="69" t="s">
+      <c r="H19" s="133"/>
+      <c r="I19" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="69" t="s">
+      <c r="J19" s="131" t="s">
         <v>29</v>
       </c>
       <c r="K19" s="25"/>
@@ -2643,27 +2819,27 @@
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
     </row>
-    <row r="20" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" s="4" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="52"/>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="80"/>
-      <c r="E20" s="78" t="s">
+      <c r="D20" s="114"/>
+      <c r="E20" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="80"/>
-      <c r="G20" s="78" t="s">
+      <c r="F20" s="114"/>
+      <c r="G20" s="113" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="80"/>
-      <c r="I20" s="63" t="s">
+      <c r="H20" s="114"/>
+      <c r="I20" s="115" t="s">
         <v>109</v>
       </c>
-      <c r="J20" s="62" t="s">
+      <c r="J20" s="116" t="s">
         <v>108</v>
       </c>
       <c r="K20" s="25"/>
@@ -2673,27 +2849,27 @@
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="78" t="s">
+      <c r="C21" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="79"/>
-      <c r="E21" s="82" t="s">
+      <c r="D21" s="117"/>
+      <c r="E21" s="118" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="83"/>
-      <c r="G21" s="82" t="s">
+      <c r="F21" s="119"/>
+      <c r="G21" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="83"/>
-      <c r="I21" s="64" t="s">
+      <c r="H21" s="119"/>
+      <c r="I21" s="120" t="s">
         <v>109</v>
       </c>
-      <c r="J21" s="62" t="s">
+      <c r="J21" s="116" t="s">
         <v>108</v>
       </c>
       <c r="K21" s="25"/>
@@ -2703,27 +2879,27 @@
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
     </row>
-    <row r="22" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" s="4" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52"/>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="122" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="79"/>
-      <c r="E22" s="82" t="s">
+      <c r="D22" s="123"/>
+      <c r="E22" s="124" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="83"/>
-      <c r="G22" s="82" t="s">
+      <c r="F22" s="125"/>
+      <c r="G22" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="83"/>
-      <c r="I22" s="64" t="s">
+      <c r="H22" s="125"/>
+      <c r="I22" s="126" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="62" t="s">
+      <c r="J22" s="127" t="s">
         <v>108</v>
       </c>
       <c r="K22" s="25"/>
@@ -2734,16 +2910,16 @@
       <c r="U22" s="5"/>
     </row>
     <row r="23" spans="1:21" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="52"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="62"/>
+      <c r="A23" s="106"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="110"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="108"/>
+      <c r="I23" s="111"/>
+      <c r="J23" s="111"/>
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
       <c r="R23" s="5"/>
@@ -2765,12 +2941,12 @@
       <c r="K24" s="26"/>
       <c r="L24" s="22"/>
     </row>
-    <row r="25" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="22"/>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="129" t="s">
         <v>104</v>
       </c>
       <c r="D25" s="26"/>
@@ -2783,12 +2959,12 @@
       <c r="K25" s="26"/>
       <c r="L25" s="22"/>
     </row>
-    <row r="26" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="22"/>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="76">
+      <c r="C26" s="130">
         <v>43613</v>
       </c>
       <c r="D26" s="26"/>
@@ -2887,16 +3063,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
@@ -2911,16 +3087,16 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:I11"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2934,7 +3110,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2943,7 +3119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -3027,7 +3203,7 @@
       <c r="A10" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="72" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3035,7 +3211,7 @@
       <c r="A11" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="72" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3051,10 +3227,10 @@
       <c r="A15" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="107"/>
+      <c r="C15" s="96"/>
       <c r="D15" s="39"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -3078,31 +3254,31 @@
       </c>
     </row>
     <row r="24" spans="1:20" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="67" t="s">
+      <c r="D24" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="68" t="s">
+      <c r="E24" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="68" t="s">
+      <c r="F24" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="68" t="s">
+      <c r="H24" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="68" t="s">
+      <c r="I24" s="65" t="s">
         <v>43</v>
       </c>
       <c r="Q24" s="42"/>
@@ -3424,7 +3600,7 @@
       <c r="A10" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="72" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3432,7 +3608,7 @@
       <c r="A11" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="72" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3448,11 +3624,11 @@
       <c r="A15" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="73"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="69"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
@@ -3475,31 +3651,31 @@
       </c>
     </row>
     <row r="24" spans="1:20" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="67" t="s">
+      <c r="D24" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="68" t="s">
+      <c r="E24" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="68" t="s">
+      <c r="F24" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="68" t="s">
+      <c r="H24" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="68" t="s">
+      <c r="I24" s="65" t="s">
         <v>43</v>
       </c>
       <c r="Q24" s="42"/>
@@ -3820,7 +3996,7 @@
       <c r="A10" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="72" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3828,7 +4004,7 @@
       <c r="A11" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="72" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3844,10 +4020,10 @@
       <c r="A15" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="107"/>
+      <c r="C15" s="96"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
@@ -3870,28 +4046,28 @@
       </c>
     </row>
     <row r="24" spans="1:19" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="68" t="s">
+      <c r="D24" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="68" t="s">
+      <c r="E24" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="68" t="s">
+      <c r="F24" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="68" t="s">
+      <c r="H24" s="65" t="s">
         <v>43</v>
       </c>
       <c r="P24" s="42"/>
@@ -4131,21 +4307,21 @@
   <sheetData>
     <row r="1" spans="1:6" s="16" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="66"/>
-      <c r="B2" s="108" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="110"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="99"/>
     </row>
     <row r="3" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="111"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="113"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="102"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
@@ -4340,31 +4516,31 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="14"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="114"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="115" t="s">
+      <c r="B23" s="104" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="116" t="s">
+      <c r="D23" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="116"/>
-      <c r="F23" s="116"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="115"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="116"/>
-      <c r="E24" s="116"/>
-      <c r="F24" s="116"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B27" s="12"/>

</xml_diff>